<commit_message>
fix spelling of report sheet names
</commit_message>
<xml_diff>
--- a/src/api/reports/templates/benthiclit_summary.xlsx
+++ b/src/api/reports/templates/benthiclit_summary.xlsx
@@ -9,9 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Benthi LIT SE" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Benthi LIT SU" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Benthi LIT Obs" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Benthic LIT SE" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Benthic LIT SU" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Benthic LIT Obs" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Charts" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -132,7 +132,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
@@ -172,7 +172,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74"/>
@@ -291,7 +291,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74"/>
@@ -394,7 +394,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74"/>
@@ -845,7 +845,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
add coming soon message to xlsx templates
</commit_message>
<xml_diff>
--- a/src/api/reports/templates/benthiclit_summary.xlsx
+++ b/src/api/reports/templates/benthiclit_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">Automatically generated chart(s) coming soon to this tab.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -128,11 +136,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17"/>
@@ -172,7 +180,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74"/>
@@ -291,7 +299,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74"/>
@@ -394,7 +402,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="74"/>
@@ -841,12 +849,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>